<commit_message>
Create Customer within Loan IQ
GDE-8452

Change sheet name and add column in dataset
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ04_BaselineNonAgentSyndication.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ04_BaselineNonAgentSyndication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7B9510-ED11-4AC7-BB61-D6EF765C1FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECC2013-CA81-4BB1-9AE2-1E675128F949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRED01_DealSetup" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="1008">
   <si>
     <t>rowid</t>
   </si>
@@ -3061,6 +3061,9 @@
   </si>
   <si>
     <t>ESPS1 7120655</t>
+  </si>
+  <si>
+    <t>Borrower1_LegalName</t>
   </si>
 </sst>
 </file>
@@ -9286,10 +9289,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AK17"/>
+  <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9300,30 +9303,30 @@
     <col min="4" max="4" width="25.140625" style="20" customWidth="1"/>
     <col min="5" max="7" width="24" style="20" customWidth="1"/>
     <col min="8" max="9" width="34.28515625" style="20" customWidth="1"/>
-    <col min="10" max="11" width="24" style="20" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" style="20" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="20" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="20" customWidth="1"/>
-    <col min="18" max="18" width="28.7109375" style="20" customWidth="1"/>
-    <col min="19" max="19" width="23" style="20" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="20" customWidth="1"/>
-    <col min="21" max="21" width="30.28515625" style="20" customWidth="1"/>
-    <col min="22" max="22" width="27.7109375" style="20" customWidth="1"/>
-    <col min="23" max="23" width="22.85546875" style="20" customWidth="1"/>
-    <col min="24" max="24" width="26.85546875" style="20" customWidth="1"/>
-    <col min="25" max="25" width="37.140625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="25" style="20" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" style="20" customWidth="1"/>
-    <col min="28" max="28" width="32.7109375" style="20" customWidth="1"/>
-    <col min="29" max="30" width="34" style="20" customWidth="1"/>
-    <col min="31" max="36" width="31.85546875" style="20" customWidth="1"/>
-    <col min="37" max="37" width="25.85546875" style="78" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="24" style="20" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="20" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" style="20" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="20" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="28.7109375" style="20" customWidth="1"/>
+    <col min="20" max="20" width="23" style="20" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375" style="20" customWidth="1"/>
+    <col min="22" max="22" width="30.28515625" style="20" customWidth="1"/>
+    <col min="23" max="23" width="27.7109375" style="20" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" style="20" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" style="20" customWidth="1"/>
+    <col min="26" max="26" width="37.140625" style="20" customWidth="1"/>
+    <col min="27" max="27" width="25" style="20" customWidth="1"/>
+    <col min="28" max="28" width="19.85546875" style="20" customWidth="1"/>
+    <col min="29" max="29" width="32.7109375" style="20" customWidth="1"/>
+    <col min="30" max="31" width="34" style="20" customWidth="1"/>
+    <col min="32" max="37" width="31.85546875" style="20" customWidth="1"/>
+    <col min="38" max="38" width="25.85546875" style="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="15" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="15" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -9354,89 +9357,92 @@
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>387</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>389</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>400</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>401</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AL1" s="15" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>156</v>
       </c>
@@ -9467,89 +9473,90 @@
       <c r="J2" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="62" t="s">
         <v>274</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="M2" s="60" t="s">
         <v>413</v>
       </c>
-      <c r="M2" s="62" t="s">
+      <c r="N2" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="N2" s="62" t="s">
+      <c r="O2" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="O2" s="62" t="s">
+      <c r="P2" s="62" t="s">
         <v>414</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="60" t="s">
+      <c r="R2" s="60" t="s">
         <v>273</v>
       </c>
-      <c r="R2" s="62" t="s">
+      <c r="S2" s="62" t="s">
         <v>415</v>
       </c>
-      <c r="S2" s="62" t="s">
+      <c r="T2" s="62" t="s">
         <v>416</v>
       </c>
-      <c r="T2" s="62" t="s">
+      <c r="U2" s="62" t="s">
         <v>417</v>
       </c>
-      <c r="U2" s="62" t="s">
+      <c r="V2" s="62" t="s">
         <v>418</v>
       </c>
-      <c r="V2" s="62" t="s">
+      <c r="W2" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="X2" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="X2" s="62" t="s">
+      <c r="Y2" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="Z2" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="AA2" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AB2" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="AB2" s="62" t="s">
+      <c r="AC2" s="62" t="s">
         <v>423</v>
       </c>
-      <c r="AC2" s="62" t="s">
+      <c r="AD2" s="62" t="s">
         <v>424</v>
       </c>
-      <c r="AD2" s="62" t="s">
+      <c r="AE2" s="62" t="s">
         <v>425</v>
       </c>
-      <c r="AE2" s="62" t="s">
+      <c r="AF2" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AG2" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="AG2" s="23" t="s">
+      <c r="AH2" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="AK2" s="23" t="s">
+      <c r="AL2" s="23" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="G16" s="32"/>
       <c r="I16" s="33"/>
     </row>
@@ -9571,7 +9578,7 @@
   </sheetPr>
   <dimension ref="A1:CY2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AX1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BB5" sqref="BB5"/>
     </sheetView>

</xml_diff>